<commit_message>
Adding static class RandomGenerator
</commit_message>
<xml_diff>
--- a/GroceryStoryTraffic/visitPattern_v0.xlsx
+++ b/GroceryStoryTraffic/visitPattern_v0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rchang/Google Drive/CS/NEU/5500_SEFoundation/project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yfyan\Desktop\NEU\Summer_2020\cs5500\cs5500_sum2020_group8\GroceryStoryTraffic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{078DE9FD-4431-C94B-9158-DB1299B6E6AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59BB1AFB-A9CD-4BEF-9ED7-2BC3367292FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6060" yWindow="1320" windowWidth="24780" windowHeight="16620" xr2:uid="{F49934F5-27AF-1742-B684-4A730E0570D6}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{F49934F5-27AF-1742-B684-4A730E0570D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Assumption notes" sheetId="4" r:id="rId1"/>
@@ -654,9 +654,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -684,19 +681,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -707,13 +695,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -744,12 +726,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -766,6 +742,30 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1089,11 +1089,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36476272-BF62-AB49-8A53-B32AA3F0E4B1}">
   <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A21" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="35.83203125" customWidth="1"/>
     <col min="2" max="2" width="23.1640625" customWidth="1"/>
@@ -1103,17 +1103,17 @@
     <col min="6" max="6" width="44.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="28" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:11" ht="27.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="62" t="s">
         <v>109</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-    </row>
-    <row r="2" spans="1:11" ht="23" x14ac:dyDescent="0.2">
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+    </row>
+    <row r="2" spans="1:11" ht="23" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>25</v>
       </c>
@@ -1125,7 +1125,7 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:11" ht="23" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="23" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>26</v>
       </c>
@@ -1140,7 +1140,7 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -1153,23 +1153,23 @@
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="23" t="s">
+    <row r="5" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="24" t="s">
+      <c r="D5" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="24" t="s">
+      <c r="E5" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="F5" s="25" t="s">
+      <c r="F5" s="21" t="s">
         <v>38</v>
       </c>
       <c r="G5" s="7"/>
@@ -1178,64 +1178,64 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:11" ht="20" x14ac:dyDescent="0.2">
-      <c r="A6" s="13" t="s">
+    <row r="6" spans="1:11" ht="20.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="F6" s="14"/>
+      <c r="F6" s="13"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:11" ht="20" x14ac:dyDescent="0.2">
-      <c r="A7" s="13" t="s">
+    <row r="7" spans="1:11" ht="20.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="E7" s="9"/>
-      <c r="F7" s="14"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="13"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:11" ht="20" x14ac:dyDescent="0.2">
-      <c r="A8" s="13" t="s">
+    <row r="8" spans="1:11" ht="20.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="E8" s="9"/>
-      <c r="F8" s="14" t="s">
+      <c r="E8" s="8"/>
+      <c r="F8" s="13" t="s">
         <v>39</v>
       </c>
       <c r="H8" s="1"/>
@@ -1243,21 +1243,21 @@
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
     </row>
-    <row r="9" spans="1:11" ht="20" x14ac:dyDescent="0.2">
-      <c r="A9" s="13" t="s">
+    <row r="9" spans="1:11" ht="20.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="9" t="s">
+      <c r="C9" s="10"/>
+      <c r="D9" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="F9" s="14" t="s">
+      <c r="F9" s="13" t="s">
         <v>51</v>
       </c>
       <c r="H9" s="1"/>
@@ -1265,21 +1265,21 @@
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="1:11" ht="63" x14ac:dyDescent="0.2">
-      <c r="A10" s="13" t="s">
+    <row r="10" spans="1:11" ht="61.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="11"/>
-      <c r="D10" s="9" t="s">
+      <c r="C10" s="10"/>
+      <c r="D10" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="F10" s="15" t="s">
+      <c r="F10" s="14" t="s">
         <v>83</v>
       </c>
       <c r="H10" s="1"/>
@@ -1287,19 +1287,19 @@
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:11" ht="20" x14ac:dyDescent="0.2">
-      <c r="A11" s="13" t="s">
+    <row r="11" spans="1:11" ht="20.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9" t="s">
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="F11" s="30" t="s">
+      <c r="F11" s="24" t="s">
         <v>84</v>
       </c>
       <c r="H11" s="1"/>
@@ -1307,19 +1307,19 @@
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
     </row>
-    <row r="12" spans="1:11" ht="20" x14ac:dyDescent="0.2">
-      <c r="A12" s="32" t="s">
+    <row r="12" spans="1:11" ht="20.5" x14ac:dyDescent="0.45">
+      <c r="A12" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="33">
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="27">
         <v>0.15</v>
       </c>
-      <c r="F12" s="30" t="s">
+      <c r="F12" s="24" t="s">
         <v>88</v>
       </c>
       <c r="H12" s="1"/>
@@ -1327,19 +1327,19 @@
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="1:11" ht="21" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="16" t="s">
+    <row r="13" spans="1:11" ht="21" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17" t="s">
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="F13" s="31" t="s">
+      <c r="F13" s="25" t="s">
         <v>85</v>
       </c>
       <c r="H13" s="1"/>
@@ -1347,114 +1347,114 @@
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
     </row>
-    <row r="16" spans="1:11" ht="28" x14ac:dyDescent="0.3">
-      <c r="A16" s="8" t="s">
+    <row r="16" spans="1:11" ht="27.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="62" t="s">
         <v>55</v>
       </c>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
+      <c r="B16" s="62"/>
+      <c r="C16" s="62"/>
+      <c r="D16" s="62"/>
+      <c r="E16" s="62"/>
+      <c r="F16" s="62"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
     </row>
-    <row r="17" spans="1:11" s="3" customFormat="1" ht="37" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="21" t="s">
+    <row r="17" spans="1:11" s="3" customFormat="1" ht="37" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A17" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="B17" s="21" t="s">
+      <c r="B17" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="22" t="s">
+      <c r="C17" s="58" t="s">
         <v>54</v>
       </c>
-      <c r="D17" s="22"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="22"/>
+      <c r="D17" s="58"/>
+      <c r="E17" s="58"/>
+      <c r="F17" s="58"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
     </row>
-    <row r="18" spans="1:11" ht="43" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="20" t="s">
+    <row r="18" spans="1:11" ht="43" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="60" t="s">
         <v>80</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="C18" s="59" t="s">
         <v>59</v>
       </c>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
+      <c r="D18" s="59"/>
+      <c r="E18" s="59"/>
+      <c r="F18" s="59"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
     </row>
-    <row r="19" spans="1:11" ht="43" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="20"/>
+    <row r="19" spans="1:11" ht="43" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="60"/>
       <c r="B19" s="2"/>
-      <c r="C19" s="18" t="s">
+      <c r="C19" s="59" t="s">
         <v>60</v>
       </c>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
+      <c r="D19" s="59"/>
+      <c r="E19" s="59"/>
+      <c r="F19" s="59"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
     </row>
-    <row r="20" spans="1:11" s="28" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="20" t="s">
+    <row r="20" spans="1:11" s="23" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A20" s="60" t="s">
         <v>66</v>
       </c>
-      <c r="B20" s="26" t="s">
+      <c r="B20" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="C20" s="27" t="s">
+      <c r="C20" s="57" t="s">
         <v>68</v>
       </c>
-      <c r="D20" s="27"/>
-      <c r="E20" s="27"/>
-      <c r="F20" s="27"/>
-    </row>
-    <row r="21" spans="1:11" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="20"/>
+      <c r="D20" s="57"/>
+      <c r="E20" s="57"/>
+      <c r="F20" s="57"/>
+    </row>
+    <row r="21" spans="1:11" ht="40" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A21" s="60"/>
       <c r="B21" s="6"/>
-      <c r="C21" s="18" t="s">
+      <c r="C21" s="59" t="s">
         <v>69</v>
       </c>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-    </row>
-    <row r="22" spans="1:11" ht="20" x14ac:dyDescent="0.2">
-      <c r="A22" s="20"/>
+      <c r="D21" s="59"/>
+      <c r="E21" s="59"/>
+      <c r="F21" s="59"/>
+    </row>
+    <row r="22" spans="1:11" ht="20.5" x14ac:dyDescent="0.45">
+      <c r="A22" s="60"/>
       <c r="B22" s="6" t="s">
         <v>70</v>
       </c>
@@ -1465,8 +1465,8 @@
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
     </row>
-    <row r="23" spans="1:11" ht="20" x14ac:dyDescent="0.2">
-      <c r="A23" s="20"/>
+    <row r="23" spans="1:11" ht="20.5" x14ac:dyDescent="0.45">
+      <c r="A23" s="60"/>
       <c r="B23" s="6" t="s">
         <v>1</v>
       </c>
@@ -1477,33 +1477,33 @@
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
     </row>
-    <row r="24" spans="1:11" ht="20" x14ac:dyDescent="0.2">
-      <c r="A24" s="29" t="s">
+    <row r="24" spans="1:11" ht="20.5" x14ac:dyDescent="0.45">
+      <c r="A24" s="61" t="s">
         <v>81</v>
       </c>
-      <c r="B24" s="26" t="s">
+      <c r="B24" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="C24" s="26" t="s">
+      <c r="C24" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="D24" s="26"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="26"/>
-    </row>
-    <row r="25" spans="1:11" ht="20" x14ac:dyDescent="0.2">
-      <c r="A25" s="29"/>
-      <c r="B25" s="26" t="s">
+      <c r="D24" s="22"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="22"/>
+    </row>
+    <row r="25" spans="1:11" ht="20.5" x14ac:dyDescent="0.45">
+      <c r="A25" s="61"/>
+      <c r="B25" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="C25" s="26" t="s">
+      <c r="C25" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="D25" s="26"/>
-      <c r="E25" s="26"/>
-      <c r="F25" s="26"/>
-    </row>
-    <row r="26" spans="1:11" ht="20" x14ac:dyDescent="0.2">
+      <c r="D25" s="22"/>
+      <c r="E25" s="22"/>
+      <c r="F25" s="22"/>
+    </row>
+    <row r="26" spans="1:11" ht="20.5" x14ac:dyDescent="0.45">
       <c r="A26" s="6"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
@@ -1511,7 +1511,7 @@
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
     </row>
-    <row r="27" spans="1:11" ht="20" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" ht="20.5" x14ac:dyDescent="0.45">
       <c r="A27" s="6"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
@@ -1519,7 +1519,7 @@
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
     </row>
-    <row r="28" spans="1:11" ht="20" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" ht="20.5" x14ac:dyDescent="0.45">
       <c r="A28" s="6"/>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
@@ -1527,7 +1527,7 @@
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
     </row>
-    <row r="29" spans="1:11" ht="20" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" ht="20.5" x14ac:dyDescent="0.45">
       <c r="A29" s="6"/>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
@@ -1535,26 +1535,26 @@
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A30" s="19"/>
-      <c r="B30" s="19"/>
-      <c r="C30" s="19"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="19"/>
-      <c r="F30" s="19"/>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A30" s="17"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="C19:F19"/>
     <mergeCell ref="C20:F20"/>
     <mergeCell ref="C17:F17"/>
     <mergeCell ref="C21:F21"/>
     <mergeCell ref="A20:A23"/>
     <mergeCell ref="A18:A19"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A16:F16"/>
-    <mergeCell ref="C18:F18"/>
-    <mergeCell ref="C19:F19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1564,11 +1564,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83A84DD3-2ABE-3D42-8C6E-4FC495E14EE8}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="23.5" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="28" style="5" customWidth="1"/>
     <col min="2" max="2" width="19.33203125" style="5" customWidth="1"/>
@@ -1576,144 +1576,144 @@
     <col min="4" max="16384" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="26" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="52" t="s">
+    <row r="1" spans="1:3" ht="26" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="63" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-    </row>
-    <row r="2" spans="1:3" ht="25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="53"/>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-    </row>
-    <row r="3" spans="1:3" ht="25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="40" t="s">
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+    </row>
+    <row r="2" spans="1:3" ht="24" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A2" s="64"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="64"/>
+    </row>
+    <row r="3" spans="1:3" ht="24" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A3" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="41" t="s">
+      <c r="B3" s="35" t="s">
         <v>89</v>
       </c>
-      <c r="C3" s="42" t="s">
+      <c r="C3" s="36" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="43" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="44">
+      <c r="B4" s="38">
         <v>8000</v>
       </c>
-      <c r="C4" s="45">
+      <c r="C4" s="39">
         <f xml:space="preserve"> B4 * 1.15</f>
         <v>9200</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="43" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="44">
+      <c r="B5" s="38">
         <v>1000</v>
       </c>
-      <c r="C5" s="45">
+      <c r="C5" s="39">
         <f t="shared" ref="C5:C10" si="0" xml:space="preserve"> B5 * 1.15</f>
         <v>1150</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="43" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="44">
+      <c r="B6" s="38">
         <v>1200</v>
       </c>
-      <c r="C6" s="45">
+      <c r="C6" s="39">
         <f t="shared" si="0"/>
         <v>1380</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="43" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="44">
+      <c r="B7" s="38">
         <v>9000</v>
       </c>
-      <c r="C7" s="45">
+      <c r="C7" s="39">
         <f t="shared" si="0"/>
         <v>10350</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="43" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="44">
+      <c r="B8" s="38">
         <v>2500</v>
       </c>
-      <c r="C8" s="45">
+      <c r="C8" s="39">
         <f t="shared" si="0"/>
         <v>2875</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="43" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="44">
+      <c r="B9" s="38">
         <v>4000</v>
       </c>
-      <c r="C9" s="45">
+      <c r="C9" s="39">
         <f t="shared" si="0"/>
         <v>4600</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="46" t="s">
+    <row r="10" spans="1:3" ht="24" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A10" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="47">
+      <c r="B10" s="41">
         <v>5000</v>
       </c>
-      <c r="C10" s="48">
+      <c r="C10" s="42">
         <f t="shared" si="0"/>
         <v>5750</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="75" x14ac:dyDescent="0.3">
-      <c r="A11" s="49" t="s">
+    <row r="11" spans="1:3" ht="70.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="43" t="s">
         <v>90</v>
       </c>
-      <c r="B11" s="50">
+      <c r="B11" s="44">
         <f>4500 * 1.4</f>
         <v>6300</v>
       </c>
-      <c r="C11" s="45"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="43" t="s">
+      <c r="C11" s="39"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="B12" s="50">
+      <c r="B12" s="44">
         <f>4500 * 1.2</f>
         <v>5400</v>
       </c>
-      <c r="C12" s="45"/>
-    </row>
-    <row r="13" spans="1:3" ht="25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="46" t="s">
+      <c r="C12" s="39"/>
+    </row>
+    <row r="13" spans="1:3" ht="24" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A13" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="51">
+      <c r="B13" s="45">
         <f>4500 * 1.4</f>
         <v>6300</v>
       </c>
-      <c r="C13" s="48"/>
-    </row>
-    <row r="14" spans="1:3" ht="54" customHeight="1" x14ac:dyDescent="0.3"/>
+      <c r="C13" s="42"/>
+    </row>
+    <row r="14" spans="1:3" ht="54" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:C2"/>
@@ -1726,302 +1726,302 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6D3EB18-DDA3-A34F-BA5C-AF2B5A26A4E3}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="26.5" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="26.5" defaultRowHeight="21" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="16384" width="26.5" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="52" t="s">
+    <row r="1" spans="1:5" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="63" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-    </row>
-    <row r="2" spans="1:5" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="60" t="s">
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+    </row>
+    <row r="2" spans="1:5" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="C2" s="61" t="s">
+      <c r="C2" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="61" t="s">
+      <c r="D2" s="53" t="s">
         <v>40</v>
       </c>
-      <c r="E2" s="39" t="s">
+      <c r="E2" s="33" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="56" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A3" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="35">
+      <c r="B3" s="29">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="C3" s="35">
+      <c r="C3" s="29">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="D3" s="35">
+      <c r="D3" s="29">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="E3" s="34">
+      <c r="E3" s="28">
         <v>1E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="56" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A4" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="35">
+      <c r="B4" s="29">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="C4" s="35">
+      <c r="C4" s="29">
         <v>0.01</v>
       </c>
-      <c r="D4" s="35">
+      <c r="D4" s="29">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="E4" s="34">
+      <c r="E4" s="28">
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="56" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A5" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="35">
+      <c r="B5" s="29">
         <v>0.03</v>
       </c>
-      <c r="C5" s="35">
+      <c r="C5" s="29">
         <v>0.02</v>
       </c>
-      <c r="D5" s="35">
+      <c r="D5" s="29">
         <v>0.04</v>
       </c>
-      <c r="E5" s="34">
+      <c r="E5" s="28">
         <v>0.01</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="56" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A6" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="35">
+      <c r="B6" s="29">
         <v>0.05</v>
       </c>
-      <c r="C6" s="35">
+      <c r="C6" s="29">
         <v>0.03</v>
       </c>
-      <c r="D6" s="35">
+      <c r="D6" s="29">
         <v>0.06</v>
       </c>
-      <c r="E6" s="34">
+      <c r="E6" s="28">
         <v>0.05</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="56" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A7" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="35">
+      <c r="B7" s="29">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="C7" s="57">
+      <c r="C7" s="49">
         <v>0.1</v>
       </c>
-      <c r="D7" s="35">
+      <c r="D7" s="29">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="E7" s="34">
+      <c r="E7" s="28">
         <v>0.06</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="56" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A8" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="35">
+      <c r="B8" s="29">
         <v>0.08</v>
       </c>
-      <c r="C8" s="57">
+      <c r="C8" s="49">
         <v>0.1</v>
       </c>
-      <c r="D8" s="35">
+      <c r="D8" s="29">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="E8" s="34">
+      <c r="E8" s="28">
         <v>0.1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="56" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A9" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="35">
+      <c r="B9" s="29">
         <v>0.1</v>
       </c>
-      <c r="C9" s="57">
+      <c r="C9" s="49">
         <v>0.12</v>
       </c>
-      <c r="D9" s="35">
+      <c r="D9" s="29">
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="E9" s="34">
+      <c r="E9" s="28">
         <v>0.12</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="56" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A10" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="35">
+      <c r="B10" s="29">
         <v>0.08</v>
       </c>
-      <c r="C10" s="57">
+      <c r="C10" s="49">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="D10" s="35">
+      <c r="D10" s="29">
         <v>8.2000000000000003E-2</v>
       </c>
-      <c r="E10" s="34">
+      <c r="E10" s="28">
         <v>0.08</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="56" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A11" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="35">
+      <c r="B11" s="29">
         <v>0.06</v>
       </c>
-      <c r="C11" s="57">
+      <c r="C11" s="49">
         <v>0.05</v>
       </c>
-      <c r="D11" s="35">
+      <c r="D11" s="29">
         <v>0.08</v>
       </c>
-      <c r="E11" s="34">
+      <c r="E11" s="28">
         <v>0.06</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="56" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A12" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="35">
+      <c r="B12" s="29">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="C12" s="57">
+      <c r="C12" s="49">
         <v>0.06</v>
       </c>
-      <c r="D12" s="35">
+      <c r="D12" s="29">
         <v>0.09</v>
       </c>
-      <c r="E12" s="34">
+      <c r="E12" s="28">
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="56" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A13" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="35">
+      <c r="B13" s="29">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="C13" s="57">
+      <c r="C13" s="49">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="D13" s="35">
+      <c r="D13" s="29">
         <v>0.1</v>
       </c>
-      <c r="E13" s="34">
+      <c r="E13" s="28">
         <v>8.5000000000000006E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="56" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A14" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="35">
+      <c r="B14" s="29">
         <v>0.11</v>
       </c>
-      <c r="C14" s="57">
+      <c r="C14" s="49">
         <v>0.15</v>
       </c>
-      <c r="D14" s="35">
+      <c r="D14" s="29">
         <v>0.1</v>
       </c>
-      <c r="E14" s="34">
+      <c r="E14" s="28">
         <v>0.13</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="56" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A15" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="35">
+      <c r="B15" s="29">
         <v>0.12</v>
       </c>
-      <c r="C15" s="57">
+      <c r="C15" s="49">
         <v>0.12</v>
       </c>
-      <c r="D15" s="35">
+      <c r="D15" s="29">
         <v>0.09</v>
       </c>
-      <c r="E15" s="34">
+      <c r="E15" s="28">
         <v>0.15</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="56" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A16" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="35">
+      <c r="B16" s="29">
         <v>0.08</v>
       </c>
-      <c r="C16" s="57">
+      <c r="C16" s="49">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="D16" s="35">
+      <c r="D16" s="29">
         <v>0.06</v>
       </c>
-      <c r="E16" s="34">
+      <c r="E16" s="28">
         <v>0.05</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="58" t="s">
+    <row r="17" spans="1:5" ht="21.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="36">
+      <c r="B17" s="30">
         <v>0.05</v>
       </c>
-      <c r="C17" s="59">
+      <c r="C17" s="51">
         <v>0.03</v>
       </c>
-      <c r="D17" s="36">
+      <c r="D17" s="30">
         <v>0.06</v>
       </c>
-      <c r="E17" s="37">
+      <c r="E17" s="31">
         <v>0.03</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A19" s="3" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A20" s="3" t="s">
         <v>106</v>
       </c>
@@ -2038,14 +2038,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0CDC1A8-B79E-AE4D-9727-7DE3C19BEAD2}">
   <dimension ref="A1:R17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" sqref="A1:R1"/>
+      <selection pane="bottomRight" activeCell="H2" sqref="H2:K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="21" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="14.33203125" style="3" customWidth="1"/>
     <col min="2" max="2" width="14.1640625" style="3" customWidth="1"/>
@@ -2068,29 +2068,29 @@
     <col min="19" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="43" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
+    <row r="1" spans="1:18" ht="43" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="63" t="s">
         <v>108</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="52"/>
-      <c r="K1" s="52"/>
-      <c r="L1" s="52"/>
-      <c r="M1" s="52"/>
-      <c r="N1" s="52"/>
-      <c r="O1" s="52"/>
-      <c r="P1" s="52"/>
-      <c r="Q1" s="52"/>
-      <c r="R1" s="52"/>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="63"/>
+      <c r="L1" s="63"/>
+      <c r="M1" s="63"/>
+      <c r="N1" s="63"/>
+      <c r="O1" s="63"/>
+      <c r="P1" s="63"/>
+      <c r="Q1" s="63"/>
+      <c r="R1" s="63"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -2122,64 +2122,64 @@
       <c r="Q2" s="65"/>
       <c r="R2" s="65"/>
     </row>
-    <row r="3" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A3" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="62" t="s">
+      <c r="B3" s="54" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="62" t="s">
+      <c r="C3" s="54" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="62" t="s">
+      <c r="D3" s="54" t="s">
         <v>99</v>
       </c>
-      <c r="E3" s="62" t="s">
+      <c r="E3" s="54" t="s">
         <v>97</v>
       </c>
-      <c r="F3" s="62" t="s">
+      <c r="F3" s="54" t="s">
         <v>40</v>
       </c>
-      <c r="G3" s="62" t="s">
+      <c r="G3" s="54" t="s">
         <v>104</v>
       </c>
-      <c r="H3" s="63" t="s">
+      <c r="H3" s="55" t="s">
         <v>100</v>
       </c>
-      <c r="I3" s="64" t="s">
+      <c r="I3" s="56" t="s">
         <v>101</v>
       </c>
-      <c r="J3" s="63" t="s">
+      <c r="J3" s="55" t="s">
         <v>40</v>
       </c>
-      <c r="K3" s="62" t="s">
+      <c r="K3" s="54" t="s">
         <v>104</v>
       </c>
-      <c r="L3" s="63" t="s">
+      <c r="L3" s="55" t="s">
         <v>96</v>
       </c>
-      <c r="M3" s="64" t="s">
+      <c r="M3" s="56" t="s">
         <v>101</v>
       </c>
-      <c r="N3" s="63" t="s">
+      <c r="N3" s="55" t="s">
         <v>40</v>
       </c>
-      <c r="O3" s="63" t="s">
+      <c r="O3" s="55" t="s">
         <v>96</v>
       </c>
-      <c r="P3" s="64" t="s">
+      <c r="P3" s="56" t="s">
         <v>101</v>
       </c>
-      <c r="Q3" s="63" t="s">
+      <c r="Q3" s="55" t="s">
         <v>40</v>
       </c>
-      <c r="R3" s="62" t="s">
+      <c r="R3" s="54" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="54" t="s">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.5">
+      <c r="A4" s="46" t="s">
         <v>78</v>
       </c>
       <c r="B4" s="3">
@@ -2191,7 +2191,7 @@
       <c r="D4" s="3">
         <v>0.3</v>
       </c>
-      <c r="E4" s="55">
+      <c r="E4" s="47">
         <v>0.2</v>
       </c>
       <c r="F4" s="3">
@@ -2203,7 +2203,7 @@
       <c r="H4" s="3">
         <v>0.45</v>
       </c>
-      <c r="I4" s="55">
+      <c r="I4" s="47">
         <v>0.5</v>
       </c>
       <c r="J4" s="3">
@@ -2215,7 +2215,7 @@
       <c r="L4" s="3">
         <v>0.3</v>
       </c>
-      <c r="M4" s="55">
+      <c r="M4" s="47">
         <v>0.35</v>
       </c>
       <c r="N4" s="3">
@@ -2224,18 +2224,18 @@
       <c r="O4" s="3">
         <v>0.35</v>
       </c>
-      <c r="P4" s="55">
+      <c r="P4" s="47">
         <v>0.4</v>
       </c>
       <c r="Q4" s="3">
         <v>0</v>
       </c>
-      <c r="R4" s="63">
+      <c r="R4" s="55">
         <v>0.1</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="54" t="s">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.5">
+      <c r="A5" s="46" t="s">
         <v>62</v>
       </c>
       <c r="B5" s="3">
@@ -2247,7 +2247,7 @@
       <c r="D5" s="3">
         <v>0.5</v>
       </c>
-      <c r="E5" s="55">
+      <c r="E5" s="47">
         <v>0.2</v>
       </c>
       <c r="F5" s="3">
@@ -2259,7 +2259,7 @@
       <c r="H5" s="3">
         <v>0.3</v>
       </c>
-      <c r="I5" s="55">
+      <c r="I5" s="47">
         <v>0.35</v>
       </c>
       <c r="J5" s="3">
@@ -2271,7 +2271,7 @@
       <c r="L5" s="3">
         <v>0.5</v>
       </c>
-      <c r="M5" s="55">
+      <c r="M5" s="47">
         <v>0.45</v>
       </c>
       <c r="N5" s="3">
@@ -2280,18 +2280,18 @@
       <c r="O5" s="3">
         <v>0.45</v>
       </c>
-      <c r="P5" s="55">
+      <c r="P5" s="47">
         <v>0.45</v>
       </c>
       <c r="Q5" s="3">
         <v>0.02</v>
       </c>
-      <c r="R5" s="63">
+      <c r="R5" s="55">
         <v>0.3</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="54" t="s">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.5">
+      <c r="A6" s="46" t="s">
         <v>63</v>
       </c>
       <c r="B6" s="3">
@@ -2303,7 +2303,7 @@
       <c r="D6" s="3">
         <v>0.2</v>
       </c>
-      <c r="E6" s="55">
+      <c r="E6" s="47">
         <v>0.1</v>
       </c>
       <c r="F6" s="3">
@@ -2315,7 +2315,7 @@
       <c r="H6" s="3">
         <v>0.2</v>
       </c>
-      <c r="I6" s="55">
+      <c r="I6" s="47">
         <v>0.13</v>
       </c>
       <c r="J6" s="3">
@@ -2327,7 +2327,7 @@
       <c r="L6" s="3">
         <v>0.15</v>
       </c>
-      <c r="M6" s="55">
+      <c r="M6" s="47">
         <v>0.2</v>
       </c>
       <c r="N6" s="3">
@@ -2336,18 +2336,18 @@
       <c r="O6" s="3">
         <v>0.1</v>
       </c>
-      <c r="P6" s="55">
+      <c r="P6" s="47">
         <v>0.2</v>
       </c>
       <c r="Q6" s="3">
         <v>0.08</v>
       </c>
-      <c r="R6" s="63">
+      <c r="R6" s="55">
         <v>0.1</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="54" t="s">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.5">
+      <c r="A7" s="46" t="s">
         <v>64</v>
       </c>
       <c r="B7" s="3">
@@ -2359,7 +2359,7 @@
       <c r="D7" s="3">
         <v>0</v>
       </c>
-      <c r="E7" s="55">
+      <c r="E7" s="47">
         <v>0.3</v>
       </c>
       <c r="F7" s="3">
@@ -2371,7 +2371,7 @@
       <c r="H7" s="3">
         <v>0.05</v>
       </c>
-      <c r="I7" s="55">
+      <c r="I7" s="47">
         <v>0.02</v>
       </c>
       <c r="J7" s="3">
@@ -2383,7 +2383,7 @@
       <c r="L7" s="3">
         <v>0.05</v>
       </c>
-      <c r="M7" s="55">
+      <c r="M7" s="47">
         <v>0</v>
       </c>
       <c r="N7" s="3">
@@ -2392,18 +2392,18 @@
       <c r="O7" s="3">
         <v>0.05</v>
       </c>
-      <c r="P7" s="55">
+      <c r="P7" s="47">
         <v>0.15</v>
       </c>
       <c r="Q7" s="3">
         <v>0.15</v>
       </c>
-      <c r="R7" s="63">
+      <c r="R7" s="55">
         <v>0.15</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="54" t="s">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.5">
+      <c r="A8" s="46" t="s">
         <v>65</v>
       </c>
       <c r="B8" s="3">
@@ -2415,7 +2415,7 @@
       <c r="D8" s="3">
         <v>0</v>
       </c>
-      <c r="E8" s="55">
+      <c r="E8" s="47">
         <v>0.2</v>
       </c>
       <c r="F8" s="3">
@@ -2427,7 +2427,7 @@
       <c r="H8" s="3">
         <v>0</v>
       </c>
-      <c r="I8" s="55">
+      <c r="I8" s="47">
         <v>0</v>
       </c>
       <c r="J8" s="3">
@@ -2439,7 +2439,7 @@
       <c r="L8" s="3">
         <v>0</v>
       </c>
-      <c r="M8" s="55">
+      <c r="M8" s="47">
         <v>0</v>
       </c>
       <c r="N8" s="3">
@@ -2448,17 +2448,17 @@
       <c r="O8" s="3">
         <v>0.05</v>
       </c>
-      <c r="P8" s="55">
+      <c r="P8" s="47">
         <v>0</v>
       </c>
       <c r="Q8" s="3">
         <v>0.45</v>
       </c>
-      <c r="R8" s="63">
+      <c r="R8" s="55">
         <v>0.2</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A9" s="3" t="s">
         <v>76</v>
       </c>
@@ -2471,7 +2471,7 @@
       <c r="D9" s="3">
         <v>0</v>
       </c>
-      <c r="E9" s="55">
+      <c r="E9" s="47">
         <v>0</v>
       </c>
       <c r="F9" s="3">
@@ -2495,7 +2495,7 @@
       <c r="L9" s="3">
         <v>0</v>
       </c>
-      <c r="M9" s="55">
+      <c r="M9" s="47">
         <v>0</v>
       </c>
       <c r="N9" s="3">
@@ -2504,32 +2504,32 @@
       <c r="O9" s="3">
         <v>0</v>
       </c>
-      <c r="P9" s="55">
+      <c r="P9" s="47">
         <v>0</v>
       </c>
       <c r="Q9" s="3">
         <v>0.3</v>
       </c>
-      <c r="R9" s="63">
+      <c r="R9" s="55">
         <v>0.15</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.5">
       <c r="B14" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.5">
       <c r="B15" s="3" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.5">
       <c r="B16" s="3" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.5">
       <c r="B17" s="3" t="s">
         <v>105</v>
       </c>

</xml_diff>